<commit_message>
Provide ATE-04 to BADAS
</commit_message>
<xml_diff>
--- a/Docs/ATS.ETX-2i100G.xlsx
+++ b/Docs/ATS.ETX-2i100G.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\ETX-2-100G\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82B639A-FE42-48F1-8A90-EF1A519E556A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FD17E4-FC5D-42B1-A0EC-51536B198E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="930" windowWidth="20895" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="23505" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Automatic Tester Specifications</t>
   </si>
@@ -134,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -142,140 +142,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -289,42 +160,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -332,14 +173,140 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -350,6 +317,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D9EEB2F-5C94-48AF-9F0E-EA6DFEBD9781}" name="Table1" displayName="Table1" ref="A13:F16" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A13:F16" xr:uid="{1D9EEB2F-5C94-48AF-9F0E-EA6DFEBD9781}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{C2E2A5F2-A009-4030-994F-38802E4548DB}" name="Serial No." dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{2F22A3BD-DE53-40E7-BB18-B757C933EDF4}" name="Duplicated by:" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{790D161F-D312-447F-9E05-509897FD86AA}" name="Duplicate Date" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{6DD4C7C4-7DE2-4E51-AC4B-35229FCEE622}" name="Approved by:" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{9DCC6E0D-A3B7-4259-8E6B-B898B0CFAA13}" name="Approval Date" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{5B462B72-B681-4D4C-9DAF-E035A293A4A3}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -615,31 +597,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -648,47 +630,47 @@
       <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="16" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="17" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="18">
+      <c r="B6" s="10"/>
+      <c r="C6" s="7">
         <v>43586</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -706,78 +688,99 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="12">
         <v>2</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="13">
         <v>44564</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="13">
         <v>44564</v>
       </c>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
         <v>3</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="13">
         <v>44752</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="13">
         <v>44754</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="12">
+        <v>4</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="13">
+        <v>45340</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="13">
+        <v>45340</v>
+      </c>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Provide ATE-05 to BADAS
</commit_message>
<xml_diff>
--- a/Docs/ATS.ETX-2i100G.xlsx
+++ b/Docs/ATS.ETX-2i100G.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\ETX-2-100G\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FD17E4-FC5D-42B1-A0EC-51536B198E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893200E1-23E4-45AC-A3E6-EC27719CBDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="23505" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Automatic Tester Specifications</t>
   </si>
@@ -163,52 +163,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -306,6 +287,25 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -320,14 +320,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D9EEB2F-5C94-48AF-9F0E-EA6DFEBD9781}" name="Table1" displayName="Table1" ref="A13:F16" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A13:F16" xr:uid="{1D9EEB2F-5C94-48AF-9F0E-EA6DFEBD9781}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D9EEB2F-5C94-48AF-9F0E-EA6DFEBD9781}" name="Table1" displayName="Table1" ref="A13:F17" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A13:F17" xr:uid="{1D9EEB2F-5C94-48AF-9F0E-EA6DFEBD9781}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C2E2A5F2-A009-4030-994F-38802E4548DB}" name="Serial No." dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{2F22A3BD-DE53-40E7-BB18-B757C933EDF4}" name="Duplicated by:" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{790D161F-D312-447F-9E05-509897FD86AA}" name="Duplicate Date" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{6DD4C7C4-7DE2-4E51-AC4B-35229FCEE622}" name="Approved by:" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{9DCC6E0D-A3B7-4259-8E6B-B898B0CFAA13}" name="Approval Date" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{C2E2A5F2-A009-4030-994F-38802E4548DB}" name="Serial No." dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{2F22A3BD-DE53-40E7-BB18-B757C933EDF4}" name="Duplicated by:" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{790D161F-D312-447F-9E05-509897FD86AA}" name="Duplicate Date" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{6DD4C7C4-7DE2-4E51-AC4B-35229FCEE622}" name="Approved by:" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{9DCC6E0D-A3B7-4259-8E6B-B898B0CFAA13}" name="Approval Date" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{5B462B72-B681-4D4C-9DAF-E035A293A4A3}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -600,7 +600,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,14 +614,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -630,46 +630,46 @@
       <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="7">
         <v>43586</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
@@ -692,81 +692,95 @@
       <c r="A12" s="4"/>
     </row>
     <row r="13" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="8">
         <v>2</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="9">
         <v>44564</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="9">
         <v>44564</v>
       </c>
-      <c r="F14" s="14"/>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="8">
         <v>3</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="9">
         <v>44752</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="9">
         <v>44754</v>
       </c>
-      <c r="F15" s="15"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="8">
         <v>4</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="9">
         <v>45340</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="9">
         <v>45340</v>
       </c>
-      <c r="F16" s="15"/>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>5</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="9">
+        <v>45343</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="9">
+        <v>45343</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>